<commit_message>
add code & modify READ.md, png and excel
</commit_message>
<xml_diff>
--- a/AHB-to-APB-Bridge-Verification/testcase_plan.xlsx
+++ b/AHB-to-APB-Bridge-Verification/testcase_plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA\code\Github\AHB-to-APB-Bridge-Verification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA\code\IC-Verification-Portfolio\AHB-to-APB-Bridge-Verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E366DB5B-CA7F-4385-AF15-5CD80A97FCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CAED41-1F89-4F93-9F9A-21DBB443700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,14 +275,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>REGISTER_WDATA=1
-HCLK、PCLK頻率比(2:1、4:1、8:1)
-HADDR={Random}
-HSIZE=word
-HWDATA={Random}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>1. 每筆傳輸的 HADDR 與 HWDATA 都被正確對應到 PADDR 與 PWDATA
 2. Bridge能正確將讀寫操作轉換成符合APB協議的讀寫操作
 3. Bridge是否正確等待PREADY回應
@@ -304,15 +296,6 @@
   </si>
   <si>
     <t>由AHB Master發起連續的、無任何等待週期 (Zero Wait-state) 的Read-after-write 寫入傳輸。</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>REGISTER_WDATA=1
-REGISTER_RDATA=1
-HCLK、PCLK頻率比(2:1、4:1、8:1)
-HADDR={Random}
-HSIZE=word
-HWDATA={Random}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -388,25 +371,42 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>1. 確認PSEL=0，停止選擇任何APB slave
+2. 確認PENABLE=0，停止當前的APB傳輸驗證
+3. 確認復位完成後可以繼續進行讀寫操作</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>隨機模式的讀取的流程中，發生error，檢查輸出訊號邏輯</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>REGISTER_RDATA=1
-HHCLK、PCLK頻率比(2:1、4:1、8:1)
+HHCLK、PCLK頻率比(2:1)
 HADDR={8'h04, 8'h08, 8'h0C, 8'h10}
 HSIZE=word
 HWDATA={Random}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1. 確認PSEL=0，停止選擇任何APB slave
-2. 確認PENABLE=0，停止當前的APB傳輸驗證
-3. 確認復位完成後可以繼續進行讀寫操作</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>隨機模式的讀取的流程中，發生error，檢查輸出訊號邏輯</t>
+    <t>REGISTER_WDATA=1
+HCLK、PCLK頻率比(2:1)
+HADDR={Random}
+HSIZE=word
+HWDATA={Random}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REGISTER_WDATA=1
+REGISTER_RDATA=1
+HCLK、PCLK頻率比(2:1)
+HADDR={Random}
+HSIZE=word
+HWDATA={Random}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -565,103 +565,103 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5607B5-1642-4126-B55A-E6CA3108193B}">
   <dimension ref="B1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,658 +971,668 @@
     </row>
     <row r="2" spans="2:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="24"/>
+      <c r="C5" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="35"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="24"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="24"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="2:13" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="24"/>
+      <c r="C9" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="24"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="24"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="2:13" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="2:13" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="24"/>
+      <c r="C13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="2:13" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="24"/>
+      <c r="C14" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="2:13" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-    </row>
-    <row r="5" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14"/>
-      <c r="C5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="13"/>
-    </row>
-    <row r="7" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="2:13" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="H15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="2:13" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
-      <c r="C9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="13"/>
-    </row>
-    <row r="10" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="2:13" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="2:13" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-    </row>
-    <row r="14" spans="2:13" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-    </row>
-    <row r="15" spans="2:13" ht="123" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9" t="s">
+      <c r="F16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-    </row>
-    <row r="16" spans="2:13" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+      <c r="G16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="9" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="J16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
     </row>
     <row r="17" spans="2:11" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
     </row>
     <row r="18" spans="2:11" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="34"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
     </row>
     <row r="19" spans="2:11" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="35"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:11" ht="27.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="35"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
     </row>
     <row r="21" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
     </row>
     <row r="22" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="31"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="31"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="F5:F7"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="L9:L11"/>
     <mergeCell ref="B12:B14"/>
@@ -1636,16 +1646,6 @@
     <mergeCell ref="K8:K11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="F9:F11"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="F5:F7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add code & modified project status
</commit_message>
<xml_diff>
--- a/AHB-to-APB-Bridge-Verification/testcase_plan.xlsx
+++ b/AHB-to-APB-Bridge-Verification/testcase_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPGA\code\IC-Verification-Portfolio\AHB-to-APB-Bridge-Verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CAED41-1F89-4F93-9F9A-21DBB443700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE912F2C-2886-488D-9764-CF4535260256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="caselist" sheetId="3" r:id="rId1"/>
@@ -386,7 +386,7 @@
   </si>
   <si>
     <t>REGISTER_RDATA=1
-HHCLK、PCLK頻率比(2:1)
+HHCLK、PCLK頻率比(2:1、4:1、8:1)
 HADDR={8'h04, 8'h08, 8'h0C, 8'h10}
 HSIZE=word
 HWDATA={Random}</t>
@@ -394,7 +394,7 @@
   </si>
   <si>
     <t>REGISTER_WDATA=1
-HCLK、PCLK頻率比(2:1)
+HCLK、PCLK頻率比(2:1、4:1、8:1)
 HADDR={Random}
 HSIZE=word
 HWDATA={Random}</t>
@@ -403,7 +403,7 @@
   <si>
     <t>REGISTER_WDATA=1
 REGISTER_RDATA=1
-HCLK、PCLK頻率比(2:1)
+HCLK、PCLK頻率比(2:1、4:1、8:1)
 HADDR={Random}
 HSIZE=word
 HWDATA={Random}</t>
@@ -606,6 +606,42 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -621,47 +657,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5607B5-1642-4126-B55A-E6CA3108193B}">
   <dimension ref="B1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,14 +971,14 @@
     </row>
     <row r="2" spans="2:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="33"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -1019,7 +1019,7 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1028,7 +1028,7 @@
       <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="21" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -1037,77 +1037,77 @@
       <c r="G4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="21" t="s">
         <v>20</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
     </row>
     <row r="5" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="24"/>
-      <c r="C5" s="28" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="25" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="21"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="33"/>
       <c r="M5" s="9"/>
     </row>
     <row r="6" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="34"/>
       <c r="M6" s="9"/>
     </row>
     <row r="7" spans="2:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="24"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="22"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="34"/>
       <c r="M7" s="9"/>
     </row>
     <row r="8" spans="2:13" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="19" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1116,7 +1116,7 @@
       <c r="D8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="21" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -1125,77 +1125,77 @@
       <c r="G8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="28" t="s">
+      <c r="K8" s="21" t="s">
         <v>33</v>
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
     <row r="9" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24"/>
-      <c r="C9" s="28" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="25" t="s">
+      <c r="E9" s="22"/>
+      <c r="F9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="21"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="33"/>
       <c r="M9" s="9"/>
     </row>
     <row r="10" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="34"/>
       <c r="M10" s="9"/>
     </row>
     <row r="11" spans="2:13" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="22"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="34"/>
       <c r="M11" s="9"/>
     </row>
     <row r="12" spans="2:13" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -1229,7 +1229,7 @@
       <c r="M12" s="9"/>
     </row>
     <row r="13" spans="2:13" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="24"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="12" t="s">
         <v>44</v>
       </c>
@@ -1261,7 +1261,7 @@
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="2:13" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="24"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="13" t="s">
         <v>49</v>
       </c>
@@ -1623,16 +1623,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="F5:F7"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="L9:L11"/>
     <mergeCell ref="B12:B14"/>
@@ -1646,6 +1636,16 @@
     <mergeCell ref="K8:K11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="F9:F11"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="F5:F7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>